<commit_message>
implemented roads in map
</commit_message>
<xml_diff>
--- a/data/lojasAssaiDiff_routetest.xlsx
+++ b/data/lojasAssaiDiff_routetest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Estudos - Web Scraping\Bases e estudos Lojas\Lojas Assaí\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC1EE14-4633-48CB-9BCD-41CE7ABC7CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF699CEC-F632-4A64-A1D7-E02A119C71BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="46">
   <si>
     <t>value</t>
   </si>
@@ -77,54 +77,6 @@
     <t>3T2022</t>
   </si>
   <si>
-    <t>Assaí Aeroporto Congonhas</t>
-  </si>
-  <si>
-    <t>Av Washington Luís, nº 5859, Santo Amaro - São Paulo/SP - 08490-525</t>
-  </si>
-  <si>
-    <t>Assaí Anhanguera</t>
-  </si>
-  <si>
-    <t>Rua Samuel Klabin</t>
-  </si>
-  <si>
-    <t>Assaí Aricanduva</t>
-  </si>
-  <si>
-    <t>Avenida Aricanduva 5555 |</t>
-  </si>
-  <si>
-    <t>Assaí Barra Funda</t>
-  </si>
-  <si>
-    <t>Avenida Marquês de São Vicente, 1.354</t>
-  </si>
-  <si>
-    <t>Assaí Casa Verde</t>
-  </si>
-  <si>
-    <t>Avenida Engenheiro Caetano Álvares, 1927</t>
-  </si>
-  <si>
-    <t>Assaí Cidade Dutra</t>
-  </si>
-  <si>
-    <t>Av. Senador Teotonio Vilela, 2.926</t>
-  </si>
-  <si>
-    <t>Assaí Fernão Dias</t>
-  </si>
-  <si>
-    <t>Rodovia Fernão Dias, s/n</t>
-  </si>
-  <si>
-    <t>Assaí Freguesia do Ó</t>
-  </si>
-  <si>
-    <t>Avenida Nossa Senhora do Ó</t>
-  </si>
-  <si>
     <t>Assaí Guaianases</t>
   </si>
   <si>
@@ -141,6 +93,84 @@
   </si>
   <si>
     <t>Av Sarg Geraldo Santa'ana</t>
+  </si>
+  <si>
+    <t>Assaí Itapevi</t>
+  </si>
+  <si>
+    <t>Rod. Engenheiro Renê Benedito da Silva, 977</t>
+  </si>
+  <si>
+    <t>Assaí Itaquera</t>
+  </si>
+  <si>
+    <t>Avenida Sylvio Torres, 190</t>
+  </si>
+  <si>
+    <t>Assaí Jaçanã</t>
+  </si>
+  <si>
+    <t>Avenida Luís Stamatis, 35</t>
+  </si>
+  <si>
+    <t>Assaí Jabaquara</t>
+  </si>
+  <si>
+    <t>Rua Taquaruçu, 79</t>
+  </si>
+  <si>
+    <t>Assaí Jacu Pêssego</t>
+  </si>
+  <si>
+    <t>Avenida Jacu Pêssego, 750</t>
+  </si>
+  <si>
+    <t>Assaí Jaguaré</t>
+  </si>
+  <si>
+    <t>Avenida Jaguaré, 925</t>
+  </si>
+  <si>
+    <t>Assaí Jaguaré Corifeu</t>
+  </si>
+  <si>
+    <t>Av Corifeu de Azevedo Marques, Jaguaré</t>
+  </si>
+  <si>
+    <t>Assaí Jaraguá/Taipas</t>
+  </si>
+  <si>
+    <t>Avenida Raimundo Pereira de Magalhães, 10.535</t>
+  </si>
+  <si>
+    <t>Assaí Nações Unidas</t>
+  </si>
+  <si>
+    <t>Av. das Nações Unidas</t>
+  </si>
+  <si>
+    <t>Assaí Nordestina</t>
+  </si>
+  <si>
+    <t>Avenida Nordestina, 3.077</t>
+  </si>
+  <si>
+    <t>Assaí Penha - Marginal Tietê</t>
+  </si>
+  <si>
+    <t>Av. Condessa Elizabeth de Robiano, 5500</t>
+  </si>
+  <si>
+    <t>Assaí Penha Tiquatira</t>
+  </si>
+  <si>
+    <t>Av. São Miguel</t>
+  </si>
+  <si>
+    <t>Assaí Raposo Tavares</t>
+  </si>
+  <si>
+    <t>Av. Mal. Fiuza de Castro</t>
   </si>
 </sst>
 </file>
@@ -212,11 +242,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Frame0" displayName="Frame0" ref="A1:H43" totalsRowShown="0">
-  <autoFilter ref="A1:H43" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H43">
-    <sortCondition ref="D1:D43"/>
-  </sortState>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Frame0" displayName="Frame0" ref="A1:H35" totalsRowShown="0">
+  <autoFilter ref="A1:H35" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="value"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Endereço"/>
@@ -518,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,16 +593,16 @@
         <v>10</v>
       </c>
       <c r="E2" s="2">
-        <v>-23.628646</v>
+        <v>-23.526843</v>
       </c>
       <c r="F2" s="2">
-        <v>-46.667667000000002</v>
+        <v>-46.396465999999997</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -592,17 +619,15 @@
         <v>10</v>
       </c>
       <c r="E3" s="2">
-        <v>-23.517199000000002</v>
+        <v>-23.542258</v>
       </c>
       <c r="F3" s="2">
-        <v>-46.726564000000003</v>
+        <v>-46.423996000000002</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -618,15 +643,17 @@
         <v>10</v>
       </c>
       <c r="E4" s="2">
-        <v>-23.563099999999999</v>
+        <v>-23.663383</v>
       </c>
       <c r="F4" s="2">
-        <v>-46.506630000000001</v>
+        <v>-46.680224000000003</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -642,10 +669,10 @@
         <v>10</v>
       </c>
       <c r="E5" s="2">
-        <v>-23.519656000000001</v>
+        <v>-23.546430999999998</v>
       </c>
       <c r="F5" s="2">
-        <v>-46.673197999999999</v>
+        <v>-46.946899999999999</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>12</v>
@@ -666,10 +693,10 @@
         <v>10</v>
       </c>
       <c r="E6" s="2">
-        <v>-23.498628</v>
+        <v>-23.553196</v>
       </c>
       <c r="F6" s="2">
-        <v>-46.664033000000003</v>
+        <v>-46.488427999999999</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>12</v>
@@ -690,10 +717,10 @@
         <v>10</v>
       </c>
       <c r="E7" s="2">
-        <v>-23.726365000000001</v>
+        <v>-23.467191</v>
       </c>
       <c r="F7" s="2">
-        <v>-46.700617000000001</v>
+        <v>-46.584729000000003</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>12</v>
@@ -714,10 +741,10 @@
         <v>10</v>
       </c>
       <c r="E8" s="2">
-        <v>-23.467832000000001</v>
+        <v>-23.641707</v>
       </c>
       <c r="F8" s="2">
-        <v>-46.572285000000001</v>
+        <v>-46.644190999999999</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>12</v>
@@ -738,17 +765,15 @@
         <v>10</v>
       </c>
       <c r="E9" s="2">
-        <v>-23.505355999999999</v>
+        <v>-23.565317</v>
       </c>
       <c r="F9" s="2">
-        <v>-46.68976</v>
+        <v>-46.446522000000002</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -764,17 +789,15 @@
         <v>10</v>
       </c>
       <c r="E10" s="2">
-        <v>-23.526843</v>
+        <v>-23.552852999999999</v>
       </c>
       <c r="F10" s="2">
-        <v>-46.396465999999997</v>
+        <v>-46.742243999999999</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -790,15 +813,17 @@
         <v>10</v>
       </c>
       <c r="E11" s="2">
-        <v>-23.542258</v>
+        <v>-23.556875000000002</v>
       </c>
       <c r="F11" s="2">
-        <v>-46.423996000000002</v>
+        <v>-46.748359000000001</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -814,67 +839,139 @@
         <v>10</v>
       </c>
       <c r="E12" s="2">
-        <v>-23.663383</v>
+        <v>-23.449862</v>
       </c>
       <c r="F12" s="2">
-        <v>-46.680224000000003</v>
+        <v>-46.722527999999997</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="2">
+        <v>-23.678526999999999</v>
+      </c>
+      <c r="F13" s="2">
+        <v>-46.695574999999998</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="2">
+        <v>-23.510605000000002</v>
+      </c>
+      <c r="F14" s="2">
+        <v>-46.430522000000003</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="2">
+        <v>-23.512795000000001</v>
+      </c>
+      <c r="F15" s="2">
+        <v>-46.553893000000002</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="2">
+        <v>-23.515934000000001</v>
+      </c>
+      <c r="F16" s="2">
+        <v>-46.518680000000003</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2">
+        <v>-23.584363</v>
+      </c>
+      <c r="F17" s="2">
+        <v>-46.747152</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
@@ -1056,86 +1153,6 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>